<commit_message>
graphs rh-yield and fix stats
</commit_message>
<xml_diff>
--- a/stats/austroplaca/month_ETR_stats_X3.xlsx
+++ b/stats/austroplaca/month_ETR_stats_X3.xlsx
@@ -445,7 +445,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B6" t="n">
         <v>11</v>
@@ -462,16 +462,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B7" t="n">
         <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>19.8735215053764</v>
+        <v>15.580376344086</v>
       </c>
       <c r="D7" t="n">
-        <v>151.6</v>
+        <v>141.7</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -479,16 +479,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>17.2716397849462</v>
+        <v>18.5020161290323</v>
       </c>
       <c r="D8" t="n">
-        <v>156.3</v>
+        <v>129.1</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -496,16 +496,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B9" t="n">
         <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>0.444642857142854</v>
+        <v>2.48020833333335</v>
       </c>
       <c r="D9" t="n">
-        <v>19.5</v>
+        <v>48.6</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -513,16 +513,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B10" t="n">
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.00381482281111117</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -530,16 +530,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B11" t="n">
         <v>12</v>
       </c>
       <c r="C11" t="n">
-        <v>15.580376344086</v>
+        <v>47.4453975682084</v>
       </c>
       <c r="D11" t="n">
-        <v>141.7</v>
+        <v>361.566</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -547,16 +547,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>18.5020161290323</v>
+        <v>41.2198884408602</v>
       </c>
       <c r="D12" t="n">
-        <v>129.1</v>
+        <v>373.394</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -564,16 +564,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B13" t="n">
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>2.48020833333335</v>
+        <v>0.5425431547619</v>
       </c>
       <c r="D13" t="n">
-        <v>48.6</v>
+        <v>46.54</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -587,10 +587,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>0.00361111111111112</v>
+        <v>0.00879305555555557</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6</v>
+        <v>1.49</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -604,10 +604,10 @@
         <v>12</v>
       </c>
       <c r="C15" t="n">
-        <v>1.625</v>
+        <v>26.4007096774193</v>
       </c>
       <c r="D15" t="n">
-        <v>151.2</v>
+        <v>489.998</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -621,10 +621,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>2.00188172043011</v>
+        <v>12.6349986559139</v>
       </c>
       <c r="D16" t="n">
-        <v>195.6</v>
+        <v>465.6</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
final changes 17th april
</commit_message>
<xml_diff>
--- a/stats/austroplaca/month_ETR_stats_X3.xlsx
+++ b/stats/austroplaca/month_ETR_stats_X3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t xml:space="preserve">min_ETR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd_ETR</t>
   </si>
 </sst>
 </file>
@@ -374,6 +377,9 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -391,6 +397,9 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
+      <c r="F2" t="n">
+        <v>0.0254991886750858</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -408,6 +417,9 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
+      <c r="F3" t="n">
+        <v>13.0484203546695</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -425,6 +437,9 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
+      <c r="F4" t="n">
+        <v>19.3580536394718</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -442,6 +457,9 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
+      <c r="F5" t="n">
+        <v>3.42081448184145</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -459,6 +477,9 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -476,6 +497,9 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
+      <c r="F7" t="n">
+        <v>25.4418999660482</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -493,6 +517,9 @@
       <c r="E8" t="n">
         <v>0</v>
       </c>
+      <c r="F8" t="n">
+        <v>21.4200597475962</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -510,6 +537,9 @@
       <c r="E9" t="n">
         <v>0</v>
       </c>
+      <c r="F9" t="n">
+        <v>7.34017452807367</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -527,6 +557,9 @@
       <c r="E10" t="n">
         <v>0</v>
       </c>
+      <c r="F10" t="n">
+        <v>0.0324652687876046</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -544,6 +577,9 @@
       <c r="E11" t="n">
         <v>0</v>
       </c>
+      <c r="F11" t="n">
+        <v>59.2576446341752</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -561,6 +597,9 @@
       <c r="E12" t="n">
         <v>0</v>
       </c>
+      <c r="F12" t="n">
+        <v>44.713832935325</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -578,6 +617,9 @@
       <c r="E13" t="n">
         <v>0</v>
       </c>
+      <c r="F13" t="n">
+        <v>3.571556864073</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -595,6 +637,9 @@
       <c r="E14" t="n">
         <v>0</v>
       </c>
+      <c r="F14" t="n">
+        <v>0.0911456381341045</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -612,6 +657,9 @@
       <c r="E15" t="n">
         <v>0</v>
       </c>
+      <c r="F15" t="n">
+        <v>53.8508294947713</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -629,6 +677,9 @@
       <c r="E16" t="n">
         <v>0</v>
       </c>
+      <c r="F16" t="n">
+        <v>42.4242775391641</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -644,6 +695,9 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>